<commit_message>
added two hds elements and more information on levels
</commit_message>
<xml_diff>
--- a/Data Files/hds_Raject.xlsx
+++ b/Data Files/hds_Raject.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10711"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12016ED3-7270-F04F-B715-604F24A1E14D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACFB9A3F-940A-374F-83AA-82F011A24EA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4800" yWindow="2300" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HDS" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12179" uniqueCount="4822">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12264" uniqueCount="4856">
   <si>
     <t>ID</t>
   </si>
@@ -15200,12 +15200,356 @@
   <si>
     <t>Acai Berry Induced Cholestatic Jaundice</t>
   </si>
+  <si>
+    <t>Polygoni Multiflori (22195249)</t>
+  </si>
+  <si>
+    <t>Polygoni Multiflori </t>
+  </si>
+  <si>
+    <t>https://pubmed.ncbi.nlm.nih.gov/22195249/</t>
+  </si>
+  <si>
+    <t>HD0302</t>
+  </si>
+  <si>
+    <t>Polygoni Multiflori (24559819)</t>
+  </si>
+  <si>
+    <t>https://pubmed.ncbi.nlm.nih.gov/24559819/</t>
+  </si>
+  <si>
+    <t>Polygoni Multiflori (20479902)</t>
+  </si>
+  <si>
+    <t>https://pubmed.ncbi.nlm.nih.gov/20479902/</t>
+  </si>
+  <si>
+    <t>Reactivation of Pulmonary Tuberculosis in a Patient with Polygonum multiflorum Thunb-Induced Hepatitis</t>
+  </si>
+  <si>
+    <t>Polygoni Multiflori (23691566)</t>
+  </si>
+  <si>
+    <t>https://pubmed.ncbi.nlm.nih.gov/23691566/</t>
+  </si>
+  <si>
+    <t>Toxic hepatitis induced by Polygonum multiflorum</t>
+  </si>
+  <si>
+    <t>Polygoni Multiflori (26379995)</t>
+  </si>
+  <si>
+    <t>https://pubmed.ncbi.nlm.nih.gov/26379995/</t>
+  </si>
+  <si>
+    <t>Acute hepatitis induced by a Chinese herbal product Qibao Meiran Wan: a case study.</t>
+  </si>
+  <si>
+    <t>HD0300</t>
+  </si>
+  <si>
+    <t>Cassiae semen</t>
+  </si>
+  <si>
+    <t>Cassia Seed, Semen Cassiae</t>
+  </si>
+  <si>
+    <t>Jue Ming Zi</t>
+  </si>
+  <si>
+    <t>决明子</t>
+  </si>
+  <si>
+    <t>Senna obtusifolia</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Senna_obtusifolia</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/thumb/8/87/Senna_obtusifolia_with_flower_and_pods.jpg/640px-Senna_obtusifolia_with_flower_and_pods.jpg</t>
+  </si>
+  <si>
+    <t>Senna obtusifolia, known by the common names Chinese senna, American sicklepod, sicklepod, etc., is a plant in the genus Senna, sometimes separated in the monotypic genus Diallobus. It grows wild in North, Central, and South America, Asia, Africa, and Oceania, and is considered a particularly serious weed in many places. It has a long-standing history of confusion with Senna tora and that taxon in many sources actually refers to the present species.</t>
+  </si>
+  <si>
+    <t>Traditional Eastern medicine,</t>
+  </si>
+  <si>
+    <t>Polygoni Multiflori Caulis</t>
+  </si>
+  <si>
+    <t>Ye Jiao Teng</t>
+  </si>
+  <si>
+    <t>Shou Wu Teng</t>
+  </si>
+  <si>
+    <t>首烏藤,夜交藤</t>
+  </si>
+  <si>
+    <t>Likelihood score: A (well established cause of clinically apparent liver injury)</t>
+  </si>
+  <si>
+    <t>Reynoutria multiflora (syn. Fallopia multiflora and Polygonum multiflorum) is a species of flowering plant in the buckwheat family Polygonaceae native to central and southern China. It is known by the English common names tuber fleeceflower and Chinese (climbing) knotweed. It is known as he shou wu in China and East Asia. Another name for the species is fo-ti, which is a misnomer. The name he shou wu means 'the black-haired Mr. He'.</t>
+  </si>
+  <si>
+    <t>Reynoutria multiflora is listed in the Chinese Pharmacopoeia and is one of the most popular perennial traditional Chinese medicines. Caution must be taken, however, as overconsumption can lead to toxicity-induced hepatitis.</t>
+  </si>
+  <si>
+    <t>Polygoni Multiflori</t>
+  </si>
+  <si>
+    <r>
+      <t>The materia medica name for the seeds in Chinese is jué míng z</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="DengXian"/>
+        <family val="4"/>
+        <charset val="134"/>
+      </rPr>
+      <t>ǐ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (simplified: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="DengXian"/>
+        <family val="4"/>
+        <charset val="134"/>
+      </rPr>
+      <t>决明子</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">; traditional: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="DengXian"/>
+        <family val="4"/>
+        <charset val="134"/>
+      </rPr>
+      <t>決明子</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>).The medicinal seeds are also known by the equivalent Korean name gyeolmyeongja (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Batang"/>
+        <family val="1"/>
+        <charset val="129"/>
+      </rPr>
+      <t>결명자</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="DengXian"/>
+        <family val="4"/>
+        <charset val="134"/>
+      </rPr>
+      <t>決明子</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) in traditional Korean medicine, and by the Japanese name ketsumei-shi (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="DengXian"/>
+        <family val="4"/>
+        <charset val="134"/>
+      </rPr>
+      <t>ケツメイシ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="DengXian"/>
+        <family val="4"/>
+        <charset val="134"/>
+      </rPr>
+      <t>決明子</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) in kamp</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="DengXian"/>
+        <family val="4"/>
+        <charset val="134"/>
+      </rPr>
+      <t>ō</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> medicine. The jue ming zi is used widely in Asia, including Southeast Asian countries such as Thailand, and its herbal tea is drunk instead of regular tea as a preventative for hypertension. It is also purported to have the ability to clear the eye. In Korea also, medicinal gyeolmyeongja is usually prepared as tea (gyeolmyeongja-cha. ‘sickle pod tea’). Senna tora (Cassia tora) is used similarly, and though distinguished in the Chinese market as the "little/lesser" variety or shao jue ming </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="DengXian"/>
+        <family val="4"/>
+        <charset val="134"/>
+      </rPr>
+      <t>小決明</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) the Japanese government's [pharmacopoeia] (Nihon yakkyokuh</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="DengXian"/>
+        <family val="4"/>
+        <charset val="134"/>
+      </rPr>
+      <t>ō</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) officially acknowledges both S. obtusifolia and S. tora to be commerced as ketsumeishi. The Japanese beverage habu-cha (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="DengXian"/>
+        <family val="4"/>
+        <charset val="134"/>
+      </rPr>
+      <t>ハブ茶</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>), as the name suggests, was originally brewed from the seeds of the habus</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="DengXian"/>
+        <family val="4"/>
+        <charset val="134"/>
+      </rPr>
+      <t>ō</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> or S. occidentalis, but currently marketed habu-cha uses S. obtusifolia as substitute, since it is a higher-yielding crop.</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -15229,6 +15573,35 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="DengXian"/>
+      <family val="4"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Batang"/>
+      <family val="1"/>
+      <charset val="129"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -15247,15 +15620,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -15568,10 +15945,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB300"/>
+  <dimension ref="A1:AB302"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="109" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R1" sqref="R1"/>
+    <sheetView tabSelected="1" topLeftCell="A266" zoomScale="109" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M300" sqref="M300"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -40963,6 +41340,175 @@
         <v>3311</v>
       </c>
     </row>
+    <row r="301" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A301" s="2" t="s">
+        <v>4837</v>
+      </c>
+      <c r="B301" s="2" t="s">
+        <v>4838</v>
+      </c>
+      <c r="C301" s="2" t="s">
+        <v>4838</v>
+      </c>
+      <c r="D301" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E301" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F301" s="2" t="s">
+        <v>4839</v>
+      </c>
+      <c r="G301" s="2" t="s">
+        <v>4840</v>
+      </c>
+      <c r="H301" s="2" t="s">
+        <v>4841</v>
+      </c>
+      <c r="I301" s="2" t="s">
+        <v>4842</v>
+      </c>
+      <c r="J301" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="K301" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="L301" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="M301" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="N301" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="O301" s="4" t="s">
+        <v>4843</v>
+      </c>
+      <c r="P301" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q301" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="R301" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="S301" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="T301" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="U301" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="V301" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="W301" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="X301" s="2" t="s">
+        <v>4844</v>
+      </c>
+      <c r="Y301" s="2" t="s">
+        <v>4845</v>
+      </c>
+      <c r="Z301" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA301" s="2" t="s">
+        <v>4846</v>
+      </c>
+      <c r="AB301" s="2" t="s">
+        <v>4855</v>
+      </c>
+    </row>
+    <row r="302" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A302" s="2" t="s">
+        <v>4825</v>
+      </c>
+      <c r="B302" s="2" t="s">
+        <v>4854</v>
+      </c>
+      <c r="C302" s="2" t="s">
+        <v>4847</v>
+      </c>
+      <c r="D302" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E302" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F302" s="2" t="s">
+        <v>4848</v>
+      </c>
+      <c r="G302" s="2" t="s">
+        <v>4849</v>
+      </c>
+      <c r="H302" s="2" t="s">
+        <v>4850</v>
+      </c>
+      <c r="J302" s="2" t="s">
+        <v>698</v>
+      </c>
+      <c r="K302" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="L302" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="M302" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="N302" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="O302" s="2" t="s">
+        <v>492</v>
+      </c>
+      <c r="P302" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q302" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="R302" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="S302" s="2" t="s">
+        <v>494</v>
+      </c>
+      <c r="T302" s="2" t="s">
+        <v>4851</v>
+      </c>
+      <c r="U302" s="2" t="s">
+        <v>495</v>
+      </c>
+      <c r="V302" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="W302" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="X302" s="4" t="s">
+        <v>496</v>
+      </c>
+      <c r="Y302" s="2" t="s">
+        <v>4852</v>
+      </c>
+      <c r="Z302" s="2" t="s">
+        <v>495</v>
+      </c>
+      <c r="AA302" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="AB302" s="2" t="s">
+        <v>4853</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:W300" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <hyperlinks>
@@ -40970,6 +41516,8 @@
     <hyperlink ref="R266" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
     <hyperlink ref="O268" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
     <hyperlink ref="R287" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="O301" r:id="rId5" xr:uid="{CB8E1394-192C-7645-B87A-BE747B84152E}"/>
+    <hyperlink ref="X302" r:id="rId6" xr:uid="{F45195C2-FEA1-9B4D-9922-C584470B9777}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="1200" verticalDpi="1200"/>
@@ -40978,10 +41526,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G512"/>
+  <dimension ref="A1:G517"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+    <sheetView topLeftCell="A481" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M506" sqref="M506"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -52755,6 +53303,121 @@
       </c>
       <c r="G512" t="s">
         <v>3896</v>
+      </c>
+    </row>
+    <row r="513" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A513" s="2" t="s">
+        <v>4822</v>
+      </c>
+      <c r="B513" s="2" t="s">
+        <v>4823</v>
+      </c>
+      <c r="C513" s="2" t="s">
+        <v>3319</v>
+      </c>
+      <c r="D513" s="2" t="s">
+        <v>4824</v>
+      </c>
+      <c r="E513" s="2">
+        <v>22195249</v>
+      </c>
+      <c r="F513" s="2" t="s">
+        <v>4825</v>
+      </c>
+      <c r="G513" s="2" t="s">
+        <v>3679</v>
+      </c>
+    </row>
+    <row r="514" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A514" s="2" t="s">
+        <v>4826</v>
+      </c>
+      <c r="B514" s="2" t="s">
+        <v>4823</v>
+      </c>
+      <c r="C514" s="2" t="s">
+        <v>3319</v>
+      </c>
+      <c r="D514" s="3" t="s">
+        <v>4827</v>
+      </c>
+      <c r="E514" s="2">
+        <v>24559819</v>
+      </c>
+      <c r="F514" s="2" t="s">
+        <v>4825</v>
+      </c>
+      <c r="G514" s="2" t="s">
+        <v>3533</v>
+      </c>
+    </row>
+    <row r="515" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A515" s="2" t="s">
+        <v>4828</v>
+      </c>
+      <c r="B515" s="2" t="s">
+        <v>4823</v>
+      </c>
+      <c r="C515" s="2" t="s">
+        <v>3319</v>
+      </c>
+      <c r="D515" s="3" t="s">
+        <v>4829</v>
+      </c>
+      <c r="E515" s="2">
+        <v>20479902</v>
+      </c>
+      <c r="F515" s="2" t="s">
+        <v>4825</v>
+      </c>
+      <c r="G515" s="2" t="s">
+        <v>4830</v>
+      </c>
+    </row>
+    <row r="516" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A516" s="2" t="s">
+        <v>4831</v>
+      </c>
+      <c r="B516" s="2" t="s">
+        <v>4823</v>
+      </c>
+      <c r="C516" s="2" t="s">
+        <v>3319</v>
+      </c>
+      <c r="D516" s="3" t="s">
+        <v>4832</v>
+      </c>
+      <c r="E516" s="2">
+        <v>23691566</v>
+      </c>
+      <c r="F516" s="2" t="s">
+        <v>4825</v>
+      </c>
+      <c r="G516" s="2" t="s">
+        <v>4833</v>
+      </c>
+    </row>
+    <row r="517" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A517" s="2" t="s">
+        <v>4834</v>
+      </c>
+      <c r="B517" s="2" t="s">
+        <v>4823</v>
+      </c>
+      <c r="C517" s="2" t="s">
+        <v>3319</v>
+      </c>
+      <c r="D517" s="3" t="s">
+        <v>4835</v>
+      </c>
+      <c r="E517" s="2">
+        <v>26379995</v>
+      </c>
+      <c r="F517" s="2" t="s">
+        <v>4825</v>
+      </c>
+      <c r="G517" s="2" t="s">
+        <v>4836</v>
       </c>
     </row>
   </sheetData>

</xml_diff>